<commit_message>
#refactor code and #fix bug multi-threading
</commit_message>
<xml_diff>
--- a/data/document/test.xlsx
+++ b/data/document/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2024\Web_Scraping_and_Trade_Market_Analysis\data\document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\github\Web_Scraping_and_Trade_Market_Analysis\data\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8408DE05-5936-4A03-ACA4-AF66E414439F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC4201C-F43F-414A-A6D7-7EB96031F5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="code" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>OTC</t>
   </si>
@@ -48,10 +48,16 @@
     <t>name</t>
   </si>
   <si>
-    <t>AAAI</t>
-  </si>
-  <si>
     <t>CTCP Bảo hiểm AAA</t>
+  </si>
+  <si>
+    <t>24H</t>
+  </si>
+  <si>
+    <t>AACORP</t>
+  </si>
+  <si>
+    <t>AAM</t>
   </si>
 </sst>
 </file>
@@ -436,20 +442,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="58.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" style="4"/>
+    <col min="1" max="1" width="12.1796875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="58.6328125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -460,18 +466,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -480,16 +486,28 @@
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="http://s.cafef.vn/hose/AAA-cong-ty-co-phan-nhua-va-moi-truong-xanh-an-phat.chn" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://s.cafef.vn/hose/AAA-cong-ty-co-phan-nhua-va-moi-truong-xanh-an-phat.chn" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A2" r:id="rId3" display="http://s.cafef.vn/otc/AAAI-ctcp-bao-hiem-aaa.chn" xr:uid="{50A86E29-4327-4BC6-8C7B-4D13B1A5398C}"/>
-    <hyperlink ref="B2" r:id="rId4" display="http://s.cafef.vn/otc/AAAI-ctcp-bao-hiem-aaa.chn" xr:uid="{54E79D64-709C-4DA7-9B17-5464A19C2DC9}"/>
+    <hyperlink ref="B3" r:id="rId1" display="http://s.cafef.vn/hose/AAA-cong-ty-co-phan-nhua-va-moi-truong-xanh-an-phat.chn" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId2" display="http://s.cafef.vn/otc/AAAI-ctcp-bao-hiem-aaa.chn" xr:uid="{54E79D64-709C-4DA7-9B17-5464A19C2DC9}"/>
+    <hyperlink ref="A2" r:id="rId3" display="http://s.cafef.vn/otc/24H-ctcp-quang-cao-truc-tuyen-24h.chn" xr:uid="{2DFD5C14-420D-4A9F-8DBF-C50F34A2657F}"/>
+    <hyperlink ref="A3" r:id="rId4" display="http://s.cafef.vn/hose/AAA-cong-ty-co-phan-nhua-va-moi-truong-xanh-an-phat.chn" xr:uid="{87229260-F3DC-4504-9BC0-D126FC1DCD8C}"/>
+    <hyperlink ref="A4" r:id="rId5" display="http://s.cafef.vn/otc/AACORP-ctcp-xay-dung-kien-truc-aa.chn" xr:uid="{BD285343-5D99-4A80-94D3-B446E006536F}"/>
+    <hyperlink ref="A5" r:id="rId6" display="http://s.cafef.vn/hose/AAM-cong-ty-co-phan-thuy-san-mekong.chn" xr:uid="{C0A3AA81-FA49-4671-8D0B-6BB49BD573DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>